<commit_message>
feat: fix kolom header dengan kolom row data yang meleset
</commit_message>
<xml_diff>
--- a/dashboard-pajak-feedback-tracker.xlsx
+++ b/dashboard-pajak-feedback-tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\alvif\projects\app-pajak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333B8637-4E12-45D2-9691-505178DF45AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E8564D-A057-47CD-BE2D-480B4163EFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{0E108306-3D9A-421D-99FA-EE6E32BB7825}"/>
+    <workbookView xWindow="5520" yWindow="150" windowWidth="11010" windowHeight="12900" xr2:uid="{0E108306-3D9A-421D-99FA-EE6E32BB7825}"/>
   </bookViews>
   <sheets>
     <sheet name="feedback" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Grade</t>
-  </si>
-  <si>
     <t xml:space="preserve">tambahkan filter multi-select </t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>rev</t>
   </si>
   <si>
-    <t>Grade:</t>
-  </si>
-  <si>
     <t>LOW</t>
   </si>
   <si>
@@ -123,6 +117,12 @@
   </si>
   <si>
     <t>Next</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Priority:</t>
   </si>
 </sst>
 </file>
@@ -599,13 +599,14 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="90.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -625,13 +626,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -639,17 +640,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -657,17 +658,17 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -675,17 +676,17 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -693,13 +694,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -707,19 +708,19 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -727,17 +728,17 @@
         <v>1</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -745,31 +746,31 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
+      <c r="B11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -777,19 +778,19 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G12" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -797,17 +798,17 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -815,13 +816,13 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: Enhance user notification system and UI improvements
- Added dynamic Echo channel scripts in master layout for user notifications.
- Display "Development Mode" badge in the navbar when in debug mode.
- Removed commented-out buttons in the dashboard view for cleaner UI.
- Improved table layout and added new columns in the pajak keluaran view.
- Updated AJAX data handling in pajak keluaran scripts to reflect new data structure.
- Introduced a new upload page for Pajak Masukan with enhanced user interaction and progress tracking.
- Created a new captcha preview page with improved token management and user feedback.
- Added new broadcast channels for user data and progress updates.
- Updated web routes to include new functionalities for CoreTax data gathering and captcha handling.
- Modified batch scripts to streamline service management for Reverb and Selenium.
- Removed obsolete stop scripts for Reverb and Queue Worker.
</commit_message>
<xml_diff>
--- a/dashboard-pajak-feedback-tracker.xlsx
+++ b/dashboard-pajak-feedback-tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\alvif\projects\app-pajak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E8564D-A057-47CD-BE2D-480B4163EFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D81EAAF-3C26-4B39-AD95-673B07C18A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5520" yWindow="150" windowWidth="11010" windowHeight="12900" xr2:uid="{0E108306-3D9A-421D-99FA-EE6E32BB7825}"/>
   </bookViews>
@@ -598,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E242C9BC-3308-4894-8CEB-4EB1B2B0620A}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +767,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>20</v>

</xml_diff>